<commit_message>
update : SOP made it shorter and removed dup info.
</commit_message>
<xml_diff>
--- a/College List/FinalList_clean.xlsx
+++ b/College List/FinalList_clean.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Futu\Git\College_publ\College List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFCB48E-B343-4A52-8615-0DC93C4293CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEF7425-78B3-40E0-B74A-182B5A67D891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -440,7 +440,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +506,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -553,7 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -573,7 +580,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -585,53 +592,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -887,15 +854,56 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
           <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -941,7 +949,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:O38" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:O38" headerRowDxfId="17">
   <autoFilter ref="A1:O38" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
     <filterColumn colId="9">
       <filters blank="1">
@@ -965,7 +973,7 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Course Name"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Sem Fee"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Sem Type"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column1" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column1" dataDxfId="16"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Uni- assi"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Research"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column2"/>
@@ -980,24 +988,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{219581C8-547A-46F3-9CE1-ED8162A58FD5}" name="Table2" displayName="Table2" ref="A1:O21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{219581C8-547A-46F3-9CE1-ED8162A58FD5}" name="Table2" displayName="Table2" ref="A1:O21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:O21" xr:uid="{219581C8-547A-46F3-9CE1-ED8162A58FD5}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{89ED7DE2-3B8D-439C-9C7A-DE8BBB7D2B9F}" name="Type of College" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{DCAB332F-C3AD-4DF8-BED6-1C8A1F2CCE44}" name="College Name" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{8652373D-D896-4250-875C-D25FFC7E1F4D}" name="Distance" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{0EDE2A9F-4866-495D-8210-DDBCEFC933CC}" name="Priority" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{5817422A-43FF-4A0D-B131-49747A5CD4A9}" name="Link" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{3D87FD33-AA39-440F-9D88-4E75EAB0EF63}" name="Restriction" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{DDB57203-6C28-4A58-9F58-6B4BC896D1D9}" name="Lang" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{CE6E25F1-76F9-4826-AE94-0BC6D5459D0A}" name="Course Type" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{4100B21E-FE90-4590-BCF5-22DC88295627}" name="Course Name" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{40D3DC05-5208-457A-93A3-788C9EFE4854}" name="Sem Fee" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{B116F834-9A2E-4803-A0B9-AE96692536FD}" name="Sem Type" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{60386A56-9E71-47C4-9B85-30839E1D3A5F}" name="Column1" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{DA1EC3FD-55B5-4CF6-A96D-24291F5AF896}" name="Uni- assi" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{89ED7DE2-3B8D-439C-9C7A-DE8BBB7D2B9F}" name="Type of College" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{DCAB332F-C3AD-4DF8-BED6-1C8A1F2CCE44}" name="College Name" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{8652373D-D896-4250-875C-D25FFC7E1F4D}" name="Distance" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{0EDE2A9F-4866-495D-8210-DDBCEFC933CC}" name="Priority" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{5817422A-43FF-4A0D-B131-49747A5CD4A9}" name="Link" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{3D87FD33-AA39-440F-9D88-4E75EAB0EF63}" name="Restriction" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{DDB57203-6C28-4A58-9F58-6B4BC896D1D9}" name="Lang" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{CE6E25F1-76F9-4826-AE94-0BC6D5459D0A}" name="Course Type" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{4100B21E-FE90-4590-BCF5-22DC88295627}" name="Course Name" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{40D3DC05-5208-457A-93A3-788C9EFE4854}" name="Sem Fee" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{B116F834-9A2E-4803-A0B9-AE96692536FD}" name="Sem Type" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{60386A56-9E71-47C4-9B85-30839E1D3A5F}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{DA1EC3FD-55B5-4CF6-A96D-24291F5AF896}" name="Uni- assi" dataDxfId="1"/>
     <tableColumn id="14" xr3:uid="{199D8EA0-E6F7-4904-A487-1D5435E2F61E}" name="Research"/>
-    <tableColumn id="15" xr3:uid="{E4793B12-0776-40D0-B5F7-5852EF70BD0A}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{E4793B12-0776-40D0-B5F7-5852EF70BD0A}" name="Column2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3662,7 +3670,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3772,7 +3780,7 @@
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="19" t="s">
         <v>71</v>
       </c>
       <c r="C3" s="13">

</xml_diff>